<commit_message>
code_update_v1 update the visualization
</commit_message>
<xml_diff>
--- a/proj_backtest_strategy/backtest_performance/optimization_results.xlsx
+++ b/proj_backtest_strategy/backtest_performance/optimization_results.xlsx
@@ -429,19 +429,19 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.1622094975682804</v>
+        <v>0.2859509529444935</v>
       </c>
       <c r="D2">
-        <v>0.004932704142179</v>
+        <v>0.01388827069144083</v>
       </c>
       <c r="E2">
-        <v>-0.008648733050217261</v>
+        <v>0.006621528401716747</v>
       </c>
       <c r="F2">
-        <v>-0.1390287012103186</v>
+        <v>-0.2238840684928703</v>
       </c>
       <c r="G2">
-        <v>0.5330055579275336</v>
+        <v>0.5325075328486121</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -452,19 +452,19 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.3258957046073425</v>
+        <v>0.5107610139011399</v>
       </c>
       <c r="D3">
-        <v>0.01770349574739343</v>
+        <v>0.03137483124467404</v>
       </c>
       <c r="E3">
-        <v>0.1684673861273955</v>
+        <v>0.1766367752656752</v>
       </c>
       <c r="F3">
-        <v>-0.1728977429614979</v>
+        <v>-0.2646734840316442</v>
       </c>
       <c r="G3">
-        <v>0.5231744766185907</v>
+        <v>0.5230118728062177</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -475,19 +475,19 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>0.6352840954645037</v>
+        <v>0.6184905866032928</v>
       </c>
       <c r="D4">
-        <v>0.03703855008490308</v>
+        <v>0.0518624791402557</v>
       </c>
       <c r="E4">
-        <v>0.2416977196900441</v>
+        <v>0.2613589834390402</v>
       </c>
       <c r="F4">
-        <v>-0.3366735923185685</v>
+        <v>-0.3990688081024865</v>
       </c>
       <c r="G4">
-        <v>0.4877776404749004</v>
+        <v>0.4883319378332514</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -498,19 +498,19 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.02448037071630951</v>
+        <v>0.04743822908319877</v>
       </c>
       <c r="D5">
-        <v>-0.003251502195268774</v>
+        <v>-0.006300419179037398</v>
       </c>
       <c r="E5">
-        <v>-0.01234904711175677</v>
+        <v>-0.002192891532154102</v>
       </c>
       <c r="F5">
-        <v>-0.1284619401954395</v>
+        <v>-0.2062872690305563</v>
       </c>
       <c r="G5">
-        <v>0.5496560163741954</v>
+        <v>0.5461301469193761</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -521,19 +521,19 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.05687791515415069</v>
+        <v>0.09285964204334098</v>
       </c>
       <c r="D6">
-        <v>0.005845065381594147</v>
+        <v>0.007732799577114901</v>
       </c>
       <c r="E6">
-        <v>0.1574352792779644</v>
+        <v>0.161427200727865</v>
       </c>
       <c r="F6">
-        <v>-0.1508334610988422</v>
+        <v>-0.2345201207183042</v>
       </c>
       <c r="G6">
-        <v>0.5419079122450067</v>
+        <v>0.5362671535811375</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -544,19 +544,19 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.3147638691140899</v>
+        <v>0.4255621319500999</v>
       </c>
       <c r="D7">
-        <v>0.02564078896371608</v>
+        <v>0.03268483639646356</v>
       </c>
       <c r="E7">
-        <v>0.2416673628998235</v>
+        <v>0.2553335297719969</v>
       </c>
       <c r="F7">
-        <v>-0.2693323895060191</v>
+        <v>-0.3487914831783068</v>
       </c>
       <c r="G7">
-        <v>0.4835938716213811</v>
+        <v>0.48340775868858</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -567,19 +567,19 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0.01212483500642941</v>
+        <v>0.02601404063028697</v>
       </c>
       <c r="D8">
-        <v>-0.001377578336134638</v>
+        <v>-0.003093420118658873</v>
       </c>
       <c r="E8">
-        <v>0.03647918619468999</v>
+        <v>0.04203266763915399</v>
       </c>
       <c r="F8">
-        <v>-0.09958594405876355</v>
+        <v>-0.1681493645975394</v>
       </c>
       <c r="G8">
-        <v>0.5616276364421017</v>
+        <v>0.5582776633267116</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -590,19 +590,19 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>0.04864001012169061</v>
+        <v>0.08358269619876381</v>
       </c>
       <c r="D9">
-        <v>0.006349669374847938</v>
+        <v>0.0100450360313335</v>
       </c>
       <c r="E9">
-        <v>0.2335038550999336</v>
+        <v>0.2362701805105318</v>
       </c>
       <c r="F9">
-        <v>-0.1150755500354841</v>
+        <v>-0.1894044383603727</v>
       </c>
       <c r="G9">
-        <v>0.5579675891071253</v>
+        <v>0.5521213756404834</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -613,19 +613,19 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>0.1802377507633932</v>
+        <v>0.2650197135655772</v>
       </c>
       <c r="D10">
-        <v>0.02073918755575094</v>
+        <v>0.0291622248711331</v>
       </c>
       <c r="E10">
-        <v>0.2677823271928511</v>
+        <v>0.2795450273609112</v>
       </c>
       <c r="F10">
-        <v>-0.2201704915159125</v>
+        <v>-0.3037864330808801</v>
       </c>
       <c r="G10">
-        <v>0.5113535441644061</v>
+        <v>0.5110144147841393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>